<commit_message>
Update to aggregate sample
</commit_message>
<xml_diff>
--- a/Samples/Repeat_Aggregation.xlsx
+++ b/Samples/Repeat_Aggregation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/John/Documents/Survey123Community/Samples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/John/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="3940" windowWidth="28800" windowHeight="11600"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="11600"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="929">
   <si>
     <t>type</t>
   </si>
@@ -2742,9 +2742,6 @@
     <t>Total Occupants</t>
   </si>
   <si>
-    <t>OldestBirthdate</t>
-  </si>
-  <si>
     <t>count(${Occupant_Name})</t>
   </si>
   <si>
@@ -2820,28 +2817,10 @@
     <t>Location</t>
   </si>
   <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>int((today() - ${Occupant_Birthdate}) div (1000 * 24 * 60 * 60 * 365.25))</t>
-  </si>
-  <si>
-    <t>min(${age})</t>
-  </si>
-  <si>
     <t>Summary (Occupants)</t>
   </si>
   <si>
     <t>Summary (Rooms)</t>
-  </si>
-  <si>
-    <t>Age of Eldest Occupant</t>
-  </si>
-  <si>
-    <t>Living room</t>
   </si>
 </sst>
 </file>
@@ -3128,6 +3107,30 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3160,30 +3163,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3267,15 +3246,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:X236" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:X236"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:X234" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:X234"/>
   <tableColumns count="24">
     <tableColumn id="1" name="type"/>
     <tableColumn id="2" name="name"/>
-    <tableColumn id="3" name="label" dataDxfId="4"/>
-    <tableColumn id="4" name="hint" dataDxfId="3"/>
+    <tableColumn id="3" name="label" dataDxfId="7"/>
+    <tableColumn id="4" name="hint" dataDxfId="6"/>
     <tableColumn id="5" name="constraint"/>
-    <tableColumn id="6" name="constraint_message" dataDxfId="2"/>
+    <tableColumn id="6" name="constraint_message" dataDxfId="5"/>
     <tableColumn id="7" name="required"/>
     <tableColumn id="20" name="required_message"/>
     <tableColumn id="8" name="appearance"/>
@@ -3609,7 +3588,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -3651,7 +3630,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -3671,11 +3650,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF22"/>
+  <dimension ref="A1:AF20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <pane xSplit="3" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.5" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3777,7 +3756,7 @@
         <v>893</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3788,7 +3767,7 @@
         <v>894</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -3840,10 +3819,10 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>932</v>
+        <v>927</v>
       </c>
     </row>
     <row r="10" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3860,140 +3839,105 @@
         <v>11</v>
       </c>
       <c r="M10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="11" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>928</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>929</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="K11" t="s">
-        <v>11</v>
-      </c>
-      <c r="M11" t="s">
-        <v>930</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>934</v>
-      </c>
-      <c r="K12" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" t="s">
-        <v>931</v>
+        <v>903</v>
       </c>
     </row>
     <row r="13" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>904</v>
+      </c>
+      <c r="B13" t="s">
+        <v>911</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>912</v>
+      </c>
+      <c r="I13" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>904</v>
+        <v>913</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>905</v>
-      </c>
-      <c r="B15" t="s">
-        <v>912</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>913</v>
-      </c>
-      <c r="I15" t="s">
-        <v>117</v>
+        <v>914</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>915</v>
       </c>
     </row>
     <row r="16" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>914</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>915</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>916</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>925</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>928</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>916</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>917</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="K18" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" t="s">
+        <v>918</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>926</v>
+        <v>919</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>933</v>
+        <v>920</v>
+      </c>
+      <c r="M19" t="s">
+        <v>921</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" t="s">
-        <v>917</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>918</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>916</v>
-      </c>
-      <c r="K20" t="s">
-        <v>11</v>
-      </c>
-      <c r="M20" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="s">
-        <v>920</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>921</v>
-      </c>
-      <c r="M21" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4008,27 +3952,28 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B22:B233 B2:B18 B20">
-    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+  <conditionalFormatting sqref="B20:B231 B2:B16 B18">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <dataValidations xWindow="732" yWindow="283" count="20">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Constraint" prompt="Can be used with integer and decimal types. Limit the range of numbers that can be entered (e.g., .&gt;0 and .&lt;100). " sqref="E237:E1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Constraint" prompt="Can be used with integer and decimal types. Limit the range of numbers that can be entered (e.g., .&gt;0 and .&lt;100). " sqref="E235:E1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Constraint" prompt="Limit the range of numbers that can be entered (e.g., .&gt;0 and .&lt;100). Can be used with all question types." sqref="E1:E234"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Label" prompt="The label will act as the question in your survey (e.g., What is your name?)." sqref="C1:C1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hint" prompt="This will act as extra information that can help to answer the survey question (e.g., Distances should be entered in miles)." sqref="D1:D1048576"/>
     <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Field Name" error="Name field must contain _x000a_ - unique values_x000a_ - no spaces or non-ascii characters_x000a_ - no reserved keywords or special symbols (these are listed on the type worksheet)." promptTitle="Database Field Name" prompt="This will be the field name in the resulting database. Eg: first_name,  survey_date. This field must contain _x000a_ - unique values_x000a_ - no spaces or non-ascii characters_x000a_ - no reserved keywords or special symbols (these are listed on the type worksheet)." sqref="B1:B1048576">
       <formula1>AND(LEN(B1)=LEN(SUBSTITUTE(B1," ","")),LEN(B1)&lt;32,COUNTIF(Reserved,B1) = 0,SUMPRODUCT(--ISNUMBER(SEARCH(Special,B1)))=0)</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Constraint Message" prompt="When the constraint conditions are not met, this message will appear to prompt a valid answer (e.g., Please enter a value from 0-100)." sqref="F1:F1048576 E11"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Constraint Message" prompt="When the constraint conditions are not met, this message will appear to prompt a valid answer (e.g., Please enter a value from 0-100)." sqref="F1:F1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default" prompt="Set the default value for this field. This will pre-populate the survey with the default value. This can either be used to save time by supplying a commonly used answer or by showing what type of answer choice is expected." sqref="J1:J1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Relevant" prompt="This gives you the ability to skip questions or make additional questions appear based on the response to a previous question. A question is made relevant by meeting the conditions in the relevant field (e.g., ${name} = 'value')." sqref="L1:L1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="media::image" prompt="Copy your image file to the 'media' subfolder for your project and enter the name of your image file here (e.g., image.jpg)." sqref="S1:S1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="media::audio" prompt="Copy your audio file to the 'media' subfolder for your project and enter the name of your audio file here (e.g., audio.mp3)." sqref="R1:R236"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="media::audio" prompt="Copy your audio file to the 'media' subfolder for your project and enter the name of your audio file here (e.g., audio.mp3)." sqref="R1:R234"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Localization - Label" prompt="Enter translations for your survey questions here. Include any further translations by creating a new column (e.g., label::Chinese). The list of languages will appear in a drop-down menu on the survey." sqref="P1:P1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Localization - Hint" prompt="Enter translations for your survey question hints here. Include any further translations by creating a new column (e.g., hint::Chinese). The list of languages will appear in a drop-down menu on the survey." sqref="Q1:Q1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Calculation" prompt="Perform calculations using the values of preceeding questions (e.g., ${number}*100). Reference the calculate field to display the result (e.g., The answer is ${calc}). " sqref="M1:M1048576"/>
@@ -4039,7 +3984,6 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="bind::esri:fieldAlias" prompt="Enter values to be used as the field alias in your feature service. This can be used to overwrite the default field alias values, which are derived from the question label." sqref="W1:W1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="body::esri:inputMask" prompt="Enter an expression to use an input mask to provide a set format for data entry in by using characters and symbols." sqref="X1:X1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="body::accuracyThreshold" prompt="Enter a numeric value for the threshold (in meters) above which geopoint results will not be accepted. Only applies to geopoint questions." sqref="T1:T1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Constraint" prompt="Limit the range of numbers that can be entered (e.g., .&gt;0 and .&lt;100). Can be used with all question types." sqref="E1:E10 E12:E236"/>
   </dataValidations>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4091,7 +4035,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4143,57 +4087,57 @@
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
+        <v>905</v>
+      </c>
+      <c r="B5" t="s">
         <v>906</v>
       </c>
-      <c r="B5" t="s">
-        <v>907</v>
-      </c>
       <c r="C5" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B6" t="s">
-        <v>935</v>
+        <v>908</v>
       </c>
       <c r="C6" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B7" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="C7" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B8" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C8" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B9" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C9" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
   </sheetData>
@@ -4212,7 +4156,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4251,7 +4195,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>